<commit_message>
Little update on config about obstacles Adding attributes to Obstacle.jave
Signed-off-by: Baudouin Duthoit <baud.duthoit@gmail.com>
</commit_message>
<xml_diff>
--- a/src/conf/obstacleCharateristics.xlsx
+++ b/src/conf/obstacleCharateristics.xlsx
@@ -18,9 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t>ID (int)</t>
-  </si>
-  <si>
     <t>Symbol (String)</t>
   </si>
   <si>
@@ -43,6 +40,9 @@
   </si>
   <si>
     <t>colision Top (1 or 0)</t>
+  </si>
+  <si>
+    <t>ID (int), position on the Sprite sheet</t>
   </si>
 </sst>
 </file>
@@ -377,7 +377,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -392,30 +392,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -438,7 +438,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <f>B2+1</f>

</xml_diff>